<commit_message>
Theme giao dien va config route cho cac controller cua admin va home
</commit_message>
<xml_diff>
--- a/thietkedb/Danh sach cac bang cua web.xlsx
+++ b/thietkedb/Danh sach cac bang cua web.xlsx
@@ -11,15 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$32</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
-  <si>
-    <t>Danh sách các bảng của website</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>STT</t>
   </si>
@@ -255,11 +255,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -564,268 +561,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>46</v>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>49</v>
+      <c r="C13" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>48</v>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>47</v>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D18">
@@ -834,68 +833,68 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>53</v>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>55</v>
+      <c r="C20" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>54</v>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D23">
@@ -904,12 +903,12 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D24">
@@ -918,12 +917,12 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D25">
@@ -932,83 +931,83 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>61</v>
+      <c r="C27" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>63</v>
+      <c r="C28" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>66</v>
+      <c r="C29" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="D29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>64</v>
+      <c r="C30" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>62</v>
+      <c r="C31" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1016,36 +1015,26 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>67</v>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
+  <autoFilter ref="A1:E32">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>